<commit_message>
BasicApp: update business data xlsx
</commit_message>
<xml_diff>
--- a/basic-application/basic-application-back/src/main/resources/init/business_data.xlsx
+++ b/basic-application/basic-application-back/src/main/resources/init/business_data.xlsx
@@ -8,10 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Authority" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="UserGroup" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="TechnicalUser" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="BasicUser" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Authority" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="UserGroup" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="TechnicalUser" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="BasicUser" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="82">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -127,6 +127,18 @@
     <t xml:space="preserve">julien.benichou@kobalt.fr</t>
   </si>
   <si>
+    <t xml:space="preserve">Renaud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rjoly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">renaud.joly@kobalt.fr</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gonzalez</t>
   </si>
   <si>
@@ -136,18 +148,6 @@
     <t xml:space="preserve">julien.gonzalez@kobalt.fr</t>
   </si>
   <si>
-    <t xml:space="preserve">Renaud</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rjoly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">renaud.joly@kobalt.fr</t>
-  </si>
-  <si>
     <t xml:space="preserve">Florian</t>
   </si>
   <si>
@@ -226,13 +226,13 @@
     <t xml:space="preserve">Chloé</t>
   </si>
   <si>
-    <t xml:space="preserve">Baffert Bui-Van</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cbaffertbuivan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chloe.baffert-buivan@kobalt.fr</t>
+    <t xml:space="preserve">Bui-Van</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cbuivan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chloe.buivan@kobalt.fr</t>
   </si>
   <si>
     <t xml:space="preserve">Aurélien</t>
@@ -257,6 +257,18 @@
   </si>
   <si>
     <t xml:space="preserve">vincent.weber@kobalt.fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foucher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rfoucher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roland.foucher@kobalt.fr</t>
   </si>
 </sst>
 </file>
@@ -368,7 +380,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -376,6 +388,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF0000FF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -441,6 +454,112 @@
 </table>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -693,10 +812,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -815,16 +934,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>22</v>
@@ -847,7 +966,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>38</v>
@@ -1159,6 +1278,38 @@
         <v>2</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1166,17 +1317,18 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="laurent.almeras@kobalt.fr"/>
     <hyperlink ref="E3" r:id="rId2" display="julien.benichou@kobalt.fr"/>
-    <hyperlink ref="E4" r:id="rId3" display="julien.gonzalez@kobalt.fr"/>
-    <hyperlink ref="E5" r:id="rId4" display="renaud.joly@kobalt.fr"/>
+    <hyperlink ref="E4" r:id="rId3" display="renaud.joly@kobalt.fr"/>
+    <hyperlink ref="E5" r:id="rId4" display="julien.gonzalez@kobalt.fr"/>
     <hyperlink ref="E6" r:id="rId5" display="florian.lacreuse@kobalt.fr"/>
     <hyperlink ref="E7" r:id="rId6" display="margot.piva@kobalt.fr"/>
     <hyperlink ref="E8" r:id="rId7" display="mathieu.palley@kobalt.fr"/>
     <hyperlink ref="E9" r:id="rId8" display="alexandre.wallois@kobalt.fr"/>
     <hyperlink ref="E10" r:id="rId9" display="corinne.fagno@kobalt.fr"/>
     <hyperlink ref="E11" r:id="rId10" display="anais.rouviere@kobalt.fr"/>
-    <hyperlink ref="E12" r:id="rId11" display="chloe.baffert-buivan@kobalt.fr"/>
+    <hyperlink ref="E12" r:id="rId11" display="chloe.buivan@kobalt.fr"/>
     <hyperlink ref="E13" r:id="rId12" display="aurelien.jolivet@kobalt.fr"/>
     <hyperlink ref="E14" r:id="rId13" display="vincent.weber@kobalt.fr"/>
+    <hyperlink ref="E15" r:id="rId14" display="roland.foucher@kobalt.fr"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1186,7 +1338,7 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
User: refactor + remove generic user entity + update email type
</commit_message>
<xml_diff>
--- a/basic-application/basic-application-back/src/main/resources/init/business_data.xlsx
+++ b/basic-application/basic-application-back/src/main/resources/init/business_data.xlsx
@@ -51,7 +51,7 @@
     <t xml:space="preserve">username</t>
   </si>
   <si>
-    <t xml:space="preserve">email</t>
+    <t xml:space="preserve">emailAddress</t>
   </si>
   <si>
     <t xml:space="preserve">password</t>
@@ -271,7 +271,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -299,11 +299,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -353,15 +348,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -402,7 +397,7 @@
     <tableColumn id="2" name="firstName"/>
     <tableColumn id="3" name="lastName"/>
     <tableColumn id="4" name="username"/>
-    <tableColumn id="5" name="email"/>
+    <tableColumn id="5" name="emailAddress"/>
     <tableColumn id="6" name="password"/>
     <tableColumn id="7" name="enabled"/>
     <tableColumn id="8" name="locale"/>
@@ -531,30 +526,30 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="82.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="82.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -577,488 +572,488 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="244" min="11" style="0" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="22.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="244" min="11" style="1" width="10.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="3" t="s">
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="3" t="s">
+      <c r="F6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="F7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="F8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="F9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="3" t="s">
+      <c r="H9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="3" t="s">
+      <c r="F10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="3" t="s">
+      <c r="F11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="F12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="3" t="s">
+      <c r="H12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="3" t="s">
+      <c r="F13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="3" t="s">
+      <c r="F14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" s="3" t="s">
+      <c r="F15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I16" s="3" t="s">
+      <c r="F16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>